<commit_message>
Body do email atualizado
</commit_message>
<xml_diff>
--- a/Desafio Python Web Scraping/webScraping.xlsx
+++ b/Desafio Python Web Scraping/webScraping.xlsx
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>apache</t>
+          <t>APACHE</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -508,7 +508,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>apache</t>
+          <t>APACHE</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -521,8 +521,10 @@
           <t>A vulnerability in the RDF/XML parser of Apache Jena allows an attacker to cause an external DTD to be retrieved. This issue affects Apache Jena version 4.4.0 and prior versions. Apache Jena 4.2.x and 4.3.x do not allow external entities.</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>9.800000000000001</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>9.8</t>
+        </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
@@ -540,7 +542,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>apache</t>
+          <t>APACHE</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -553,8 +555,10 @@
           <t>Multiple components in Apache NiFi 0.0.1 to 1.16.0 do not restrict XML External Entity references in the default configuration. The Standard Content Viewer service attempts to resolve XML External Entity references when viewing formatted XML files. The following Processors attempt to resolve XML External Entity references when configured with default property values: - EvaluateXPath - EvaluateXQuery - ValidateXml Apache NiFi flow configurations that include these Processors are vulnerable to malicious XML documents that contain Document Type Declarations with XML External Entity references. The resolution disables Document Type Declarations in the default configuration for these Processors, and disallows XML External Entity resolution in standard services.</t>
         </is>
       </c>
-      <c r="D4" t="n">
-        <v>7.5</v>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>7.5</t>
+        </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
@@ -572,7 +576,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>apache</t>
+          <t>APACHE</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -585,8 +589,10 @@
           <t>Apache Doris, prior to 1.0.0, used a hardcoded key and IV to initialize the cipher used for ldap password, which may lead to information disclosure.</t>
         </is>
       </c>
-      <c r="D5" t="n">
-        <v>7.5</v>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>7.5</t>
+        </is>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
@@ -604,7 +610,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>apache</t>
+          <t>APACHE</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -617,8 +623,10 @@
           <t>In Apache CouchDB prior to 3.2.2, an attacker can access an improperly secured default installation without authenticating and gain admin privileges. The CouchDB documentation has always made recommendations for properly securing an installation, including recommending using a firewall in front of all CouchDB installations.</t>
         </is>
       </c>
-      <c r="D6" t="n">
-        <v>9.800000000000001</v>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>9.8</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
@@ -636,7 +644,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>apache</t>
+          <t>APACHE</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -649,8 +657,10 @@
           <t>In APache APISIX before 3.13.1, the jwt-auth plugin has a security issue that leaks the user's secret key because the error message returned from the dependency lua-resty-jwt contains sensitive information.</t>
         </is>
       </c>
-      <c r="D7" t="n">
-        <v>7.5</v>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>7.5</t>
+        </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
@@ -668,7 +678,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>apache</t>
+          <t>APACHE</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -681,8 +691,10 @@
           <t>Incomplete fix for CVE-2021-3100. The Apache Log4j hotpatch package starting with log4j-cve-2021-44228-hotpatch-1.1-16 will now explicitly mimic the Linux capabilities and cgroups of the target Java process that the hotpatch is applied to.</t>
         </is>
       </c>
-      <c r="D8" t="n">
-        <v>8.800000000000001</v>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>8.8</t>
+        </is>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
@@ -700,7 +712,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>apache</t>
+          <t>APACHE</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -713,8 +725,10 @@
           <t>The Apache Log4j hotpatch package before log4j-cve-2021-44228-hotpatch-1.1-13 didn’t mimic the permissions of the JVM being patched, allowing it to escalate privileges.</t>
         </is>
       </c>
-      <c r="D9" t="n">
-        <v>8.800000000000001</v>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>8.8</t>
+        </is>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
@@ -732,7 +746,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>apache</t>
+          <t>APACHE</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -745,8 +759,10 @@
           <t>Apache Superset before 1.4.2 is vulnerable to SQL injection in chart data requests. Users should update to 1.4.2 or higher which addresses this issue.</t>
         </is>
       </c>
-      <c r="D10" t="n">
-        <v>9.800000000000001</v>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>9.8</t>
+        </is>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
@@ -764,7 +780,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>apache</t>
+          <t>APACHE</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -777,8 +793,10 @@
           <t>Subversion's mod_dav_svn is vulnerable to memory corruption. While looking up path-based authorization rules, mod_dav_svn servers may attempt to use memory which has already been freed. Affected Subversion mod_dav_svn servers 1.10.0 through 1.14.1 (inclusive). Servers that do not use mod_dav_svn are not affected.</t>
         </is>
       </c>
-      <c r="D11" t="n">
-        <v>7.5</v>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>7.5</t>
+        </is>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
@@ -796,7 +814,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>apache</t>
+          <t>APACHE</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -809,8 +827,10 @@
           <t>Apache Subversion SVN authz protected copyfrom paths regression Subversion servers reveal 'copyfrom' paths that should be hidden according to configured path-based authorization (authz) rules. When a node has been copied from a protected location, users with access to the copy can see the 'copyfrom' path of the original. This also reveals the fact that the node was copied. Only the 'copyfrom' path is revealed; not its contents. Both httpd and svnserve servers are vulnerable.</t>
         </is>
       </c>
-      <c r="D12" t="n">
-        <v>4.3</v>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
@@ -828,7 +848,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>apache</t>
+          <t>APACHE</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -841,8 +861,10 @@
           <t>The fix issued for CVE-2020-17530 was incomplete. So from Apache Struts 2.0.0 to 2.5.29, still some of the tag’s attributes could perform a double evaluation if a developer applied forced OGNL evaluation by using the %{...} syntax. Using forced OGNL evaluation on untrusted user input can lead to a Remote Code Execution and security degradation.</t>
         </is>
       </c>
-      <c r="D13" t="n">
-        <v>9.800000000000001</v>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>9.8</t>
+        </is>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>

</xml_diff>